<commit_message>
Sync 23_5: Update docs
</commit_message>
<xml_diff>
--- a/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
+++ b/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="450" windowWidth="19875" windowHeight="7335" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="450" windowWidth="19875" windowHeight="7335" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="RawIdeaAnalysis" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Requirement" sheetId="7" r:id="rId5"/>
     <sheet name="PID" sheetId="8" r:id="rId6"/>
     <sheet name="OPL" sheetId="4" r:id="rId7"/>
+    <sheet name="MCR_HardwareBuild" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Requirement!$C$2:$C$385</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="242">
   <si>
     <t>STT</t>
   </si>
@@ -677,6 +678,85 @@
   </si>
   <si>
     <t>Requirement/Descripttion</t>
+  </si>
+  <si>
+    <t>Tên thiết bị</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Khung xe MCR</t>
+  </si>
+  <si>
+    <t>Cần dò line</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>ECU trung tâm</t>
+  </si>
+  <si>
+    <t>Pin lipo +sạc</t>
+  </si>
+  <si>
+    <t>RC Servo</t>
+  </si>
+  <si>
+    <t>Mạch nguồn (5V, 3.3V)</t>
+  </si>
+  <si>
+    <t>Mạch dò line dùng cảm biến quang or Hồng ngoại</t>
+  </si>
+  <si>
+    <t>Dây điện</t>
+  </si>
+  <si>
+    <t>Bánh xe hộp số</t>
+  </si>
+  <si>
+    <t>Mạch cầu H lái  động cơ</t>
+  </si>
+  <si>
+    <t>Đường (lane)</t>
+  </si>
+  <si>
+    <t>N.A</t>
+  </si>
+  <si>
+    <t>Tự thiết kế or đặt mua</t>
+  </si>
+  <si>
+    <t>Mua</t>
+  </si>
+  <si>
+    <t>STM32F4 Disco</t>
+  </si>
+  <si>
+    <t>2200 mAh, 3C, 11.1V</t>
+  </si>
+  <si>
+    <t>Mua chung team</t>
+  </si>
+  <si>
+    <t>Cây chống mạch</t>
+  </si>
+  <si>
+    <t>Chỗ Mua</t>
+  </si>
+  <si>
+    <t>http://hshop.vn/</t>
+  </si>
+  <si>
+    <t>http://www.dientuachau.com/</t>
+  </si>
+  <si>
+    <t>Khoa</t>
+  </si>
+  <si>
+    <t>Tự thiết kế or đặt mua
+Lựa chọn công suất  phù hợp với tải</t>
   </si>
 </sst>
 </file>
@@ -723,7 +803,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,6 +831,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -919,7 +1005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -967,27 +1053,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1063,11 +1128,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5894,18 +5991,18 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E6" s="21" t="s">
@@ -5922,15 +6019,15 @@
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="16" t="s">
         <v>179</v>
       </c>
@@ -5942,35 +6039,35 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="55"/>
-      <c r="F8" s="56" t="s">
+      <c r="E8" s="48"/>
+      <c r="F8" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="54" t="s">
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="54" t="s">
+      <c r="K8" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="54" t="s">
+      <c r="L8" s="47" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="51"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="43" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="19" t="s">
@@ -5994,7 +6091,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="55"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="18" t="s">
         <v>161</v>
       </c>
@@ -6016,7 +6113,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="51"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="18" t="s">
         <v>165</v>
       </c>
@@ -6038,47 +6135,47 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="41" t="s">
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="36"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="55"/>
-      <c r="F14" s="56" t="s">
+      <c r="E14" s="48"/>
+      <c r="F14" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="44" t="s">
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="K14" s="45"/>
-      <c r="L14" s="46"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="51"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="49"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="43" t="s">
         <v>171</v>
       </c>
       <c r="F16" s="16" t="s">
@@ -6104,7 +6201,7 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="51"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="16" t="s">
         <v>207</v>
       </c>
@@ -6128,7 +6225,7 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="63" t="s">
         <v>173</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -6137,10 +6234,10 @@
       <c r="G18" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="I18" s="34"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="16" t="s">
         <v>179</v>
       </c>
@@ -6152,17 +6249,17 @@
       </c>
     </row>
     <row r="19" spans="5:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="E19" s="39"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="16" t="s">
         <v>174</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="34"/>
+      <c r="I19" s="59"/>
       <c r="J19" s="16" t="s">
         <v>195</v>
       </c>
@@ -6174,7 +6271,7 @@
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="63" t="s">
         <v>199</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -6183,10 +6280,10 @@
       <c r="G20" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="I20" s="34"/>
+      <c r="I20" s="59"/>
       <c r="J20" s="16" t="s">
         <v>179</v>
       </c>
@@ -6198,15 +6295,15 @@
       </c>
     </row>
     <row r="21" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="39"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="62"/>
       <c r="J21" s="16" t="s">
         <v>204</v>
       </c>
@@ -6215,6 +6312,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L15"/>
@@ -6230,12 +6333,6 @@
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I15"/>
     <mergeCell ref="L8:L9"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9412,8 +9509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9427,8 +9524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9532,4 +9629,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D5:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="16">
+        <v>2</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" s="16">
+        <v>4</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="16">
+        <v>3</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="16">
+        <v>4</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D10" s="16">
+        <v>5</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D11" s="16">
+        <v>6</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="16">
+        <v>2</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="16">
+        <v>7</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D13" s="16">
+        <v>8</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="16">
+        <v>9</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="16">
+        <v>10</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="16">
+        <v>11</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="16">
+        <v>12</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" s="69" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="70"/>
+      <c r="E21" s="68" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D22" s="71"/>
+      <c r="E22" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D20:D22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E20" r:id="rId1"/>
+    <hyperlink ref="E21" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sync 2_6: Add docs for Watchdog
</commit_message>
<xml_diff>
--- a/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
+++ b/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="450" windowWidth="19875" windowHeight="7335" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="510" windowWidth="19875" windowHeight="7275" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="RawIdeaAnalysis" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,8 @@
     <sheet name="Requirement" sheetId="7" r:id="rId5"/>
     <sheet name="PID" sheetId="8" r:id="rId6"/>
     <sheet name="OPL" sheetId="4" r:id="rId7"/>
-    <sheet name="MCR_HardwareBuild" sheetId="9" r:id="rId8"/>
+    <sheet name="MCR_Build" sheetId="9" r:id="rId8"/>
+    <sheet name="Drone_Build" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Requirement!$C$2:$C$385</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="261">
   <si>
     <t>STT</t>
   </si>
@@ -757,6 +758,63 @@
   <si>
     <t>Tự thiết kế or đặt mua
 Lựa chọn công suất  phù hợp với tải</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Tips, Guideline</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>https://oscarliang.com/best-flight-controller-quad-hex-copter/</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>How To Choose a Flight Controller for Mini Quad</t>
+  </si>
+  <si>
+    <t>HOW TO GET STARTED WITH DRONE RACING AND MINI QUAD FPV</t>
+  </si>
+  <si>
+    <t>https://oscarliang.com/mini-quad-racing-guide/</t>
+  </si>
+  <si>
+    <t>Read First</t>
+  </si>
+  <si>
+    <t>http://quanphongrc.vn/ct/may-bay-dieu-khien/1871/geprc-gep-tx-chimp-5-inch-210mm-carbon-fiber-frame-kit-with-pdb-led-xt60-camera-moun.html</t>
+  </si>
+  <si>
+    <t>Frame - GEPRC GEP-TX Chimp 5 Inch 210MM Carbon Fiber Frame Kit with PDB LED XT60 Camera Moun</t>
+  </si>
+  <si>
+    <t>Gía</t>
+  </si>
+  <si>
+    <t>970.000 VND</t>
+  </si>
+  <si>
+    <t>https://l.facebook.com/l.php?u=https%3A%2F%2Fworld.taobao.com%2Fitem%2F546230564665.htm%3Fspm%3Da312a.7700714.0.0.Qx6JBv%23detail&amp;h=ATMvQ0w2pTaQ0KFJK9Mk5PsS_INYF5Rdl3Tah-FGZMCbctGNBS5EeA3kh-jPaCYaVgJG75UKfI90HglB3qVXtBHbcTeGI-QYzIC8U-l-hprMTKhOqMXVjwwARzfwHK7SJhiQkvdlQg</t>
+  </si>
+  <si>
+    <t>Pixhaw set</t>
+  </si>
+  <si>
+    <t>https://oscarliang.com/mini-quad-not-blackout-qav250/</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>HobbyKing FPV250L Long Frame Drone A Mini Sized FPV Drone (kit)</t>
+  </si>
+  <si>
+    <t>https://hobbyking.com/en_us/hobbyking-fpv250l-long-frame-quad-copter-a-mini-sized-fpv-multi-rotor-kit.html?___store=en_us</t>
   </si>
 </sst>
 </file>
@@ -803,7 +861,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,6 +895,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,7 +1069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1053,6 +1117,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1155,8 +1221,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1165,6 +1229,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4579,52 +4647,6 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>323850</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7169" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s7169"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5966,11 +5988,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5991,18 +6013,18 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E6" s="21" t="s">
@@ -6019,15 +6041,15 @@
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="16" t="s">
         <v>179</v>
       </c>
@@ -6039,35 +6061,35 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="48"/>
-      <c r="F8" s="49" t="s">
+      <c r="E8" s="50"/>
+      <c r="F8" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="47" t="s">
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="47" t="s">
+      <c r="K8" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="47" t="s">
+      <c r="L8" s="49" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="44"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="45" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="19" t="s">
@@ -6091,7 +6113,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="48"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="18" t="s">
         <v>161</v>
       </c>
@@ -6113,7 +6135,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="44"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18" t="s">
         <v>165</v>
       </c>
@@ -6135,47 +6157,47 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="34" t="s">
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="35"/>
-      <c r="L13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="48"/>
-      <c r="F14" s="49" t="s">
+      <c r="E14" s="50"/>
+      <c r="F14" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="37" t="s">
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="K14" s="38"/>
-      <c r="L14" s="39"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="44"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="42"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="44"/>
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="45" t="s">
         <v>171</v>
       </c>
       <c r="F16" s="16" t="s">
@@ -6201,7 +6223,7 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="44"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="16" t="s">
         <v>207</v>
       </c>
@@ -6225,7 +6247,7 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="65" t="s">
         <v>173</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -6234,10 +6256,10 @@
       <c r="G18" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="H18" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="I18" s="59"/>
+      <c r="I18" s="61"/>
       <c r="J18" s="16" t="s">
         <v>179</v>
       </c>
@@ -6249,17 +6271,17 @@
       </c>
     </row>
     <row r="19" spans="5:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="E19" s="64"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="16" t="s">
         <v>174</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="60" t="s">
+      <c r="H19" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="59"/>
+      <c r="I19" s="61"/>
       <c r="J19" s="16" t="s">
         <v>195</v>
       </c>
@@ -6271,7 +6293,7 @@
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="65" t="s">
         <v>199</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -6280,10 +6302,10 @@
       <c r="G20" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="H20" s="58" t="s">
+      <c r="H20" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="I20" s="59"/>
+      <c r="I20" s="61"/>
       <c r="J20" s="16" t="s">
         <v>179</v>
       </c>
@@ -6295,15 +6317,15 @@
       </c>
     </row>
     <row r="21" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="64"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="G21" s="60" t="s">
+      <c r="G21" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="61"/>
-      <c r="I21" s="62"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="64"/>
       <c r="J21" s="16" t="s">
         <v>204</v>
       </c>
@@ -6335,35 +6357,6 @@
     <mergeCell ref="L8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="PDF" dvAspect="DVASPECT_ICON" shapeId="7169" r:id="rId3">
-          <objectPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="PDF" dvAspect="DVASPECT_ICON" shapeId="7169" r:id="rId3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
 </worksheet>
 </file>
 
@@ -6371,8 +6364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H385"/>
   <sheetViews>
-    <sheetView topLeftCell="C82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6385,7 +6378,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="67" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -6393,37 +6386,37 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G3" s="66"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="66"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="66"/>
+      <c r="G5" s="68"/>
       <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="66"/>
+      <c r="G6" s="68"/>
       <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="66"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="66"/>
+      <c r="G8" s="68"/>
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
@@ -9509,8 +9502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9525,7 +9518,7 @@
   <dimension ref="B4:F12"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9635,8 +9628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9648,16 +9641,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F5" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="33" t="s">
         <v>220</v>
       </c>
     </row>
@@ -9827,13 +9820,13 @@
       <c r="D20" s="69" t="s">
         <v>237</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="34" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="70"/>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="34" t="s">
         <v>239</v>
       </c>
     </row>
@@ -9853,4 +9846,286 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="72" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>8</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>9</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <v>10</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>11</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>12</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="72" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <v>2</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="16">
+        <v>3</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <v>4</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
+        <v>5</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
+        <v>6</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
+        <v>7</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>8</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
+        <v>9</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
+        <v>10</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
+        <v>11</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D20" r:id="rId1"/>
+    <hyperlink ref="D19" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E8"/>
+    <hyperlink ref="D22" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sync 4_6: First Implement for Independent Watchdog
</commit_message>
<xml_diff>
--- a/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
+++ b/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="272">
   <si>
     <t>STT</t>
   </si>
@@ -802,9 +802,6 @@
     <t>https://l.facebook.com/l.php?u=https%3A%2F%2Fworld.taobao.com%2Fitem%2F546230564665.htm%3Fspm%3Da312a.7700714.0.0.Qx6JBv%23detail&amp;h=ATMvQ0w2pTaQ0KFJK9Mk5PsS_INYF5Rdl3Tah-FGZMCbctGNBS5EeA3kh-jPaCYaVgJG75UKfI90HglB3qVXtBHbcTeGI-QYzIC8U-l-hprMTKhOqMXVjwwARzfwHK7SJhiQkvdlQg</t>
   </si>
   <si>
-    <t>Pixhaw set</t>
-  </si>
-  <si>
     <t>https://oscarliang.com/mini-quad-not-blackout-qav250/</t>
   </si>
   <si>
@@ -815,6 +812,43 @@
   </si>
   <si>
     <t>https://hobbyking.com/en_us/hobbyking-fpv250l-long-frame-quad-copter-a-mini-sized-fpv-multi-rotor-kit.html?___store=en_us</t>
+  </si>
+  <si>
+    <t>http://quanphongrc.vn/ct/may-bay-dieu-khien/1419/dalrc-dl265-fpv-quad-frame-kit.html</t>
+  </si>
+  <si>
+    <t>Loại</t>
+  </si>
+  <si>
+    <t>Khung</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>DALRC DL265 FPV Quad Frame Kit</t>
+  </si>
+  <si>
+    <t>820.000 VND</t>
+  </si>
+  <si>
+    <t>SDI FEW-250 250mm Carbon Fiber</t>
+  </si>
+  <si>
+    <t>http://quanphongrc.vn/ct/may-bay-dieu-khien/774/sdi-few-250-250mm-carbon-fiber.html</t>
+  </si>
+  <si>
+    <t>https://world.taobao.com/item/532843050547.htm?spm=a312a.7700714.0.0.M3X7BM#detail</t>
+  </si>
+  <si>
+    <t>Pixhaw set - full</t>
+  </si>
+  <si>
+    <t>Pixhaw set - Not full 1 - Tran Thanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+¥ 600.00 </t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1119,6 +1153,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,27 +1253,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,9 +1268,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4591,15 +4634,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>277091</xdr:colOff>
+      <xdr:colOff>432955</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>103910</xdr:rowOff>
+      <xdr:rowOff>86592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>63</xdr:col>
-      <xdr:colOff>145472</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>3602</xdr:rowOff>
+      <xdr:colOff>301336</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>176784</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4623,7 +4666,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="277091" y="1246910"/>
+          <a:off x="432955" y="1229592"/>
           <a:ext cx="40981745" cy="16092192"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5961,7 +6004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="N95" sqref="N95"/>
     </sheetView>
   </sheetViews>
@@ -6013,18 +6056,18 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="56" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E6" s="21" t="s">
@@ -6041,15 +6084,15 @@
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="16" t="s">
         <v>179</v>
       </c>
@@ -6061,35 +6104,35 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="50"/>
-      <c r="F8" s="51" t="s">
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="49" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="49" t="s">
+      <c r="K8" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="49" t="s">
+      <c r="L8" s="58" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="46"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="54" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="19" t="s">
@@ -6113,7 +6156,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="50"/>
+      <c r="E11" s="59"/>
       <c r="F11" s="18" t="s">
         <v>161</v>
       </c>
@@ -6135,7 +6178,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="46"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="18" t="s">
         <v>165</v>
       </c>
@@ -6157,47 +6200,47 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="36" t="s">
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="47"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="50"/>
-      <c r="F14" s="51" t="s">
+      <c r="E14" s="59"/>
+      <c r="F14" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="39" t="s">
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="K14" s="40"/>
-      <c r="L14" s="41"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="50"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="46"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="44"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="53"/>
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="54" t="s">
         <v>171</v>
       </c>
       <c r="F16" s="16" t="s">
@@ -6223,7 +6266,7 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="46"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="16" t="s">
         <v>207</v>
       </c>
@@ -6247,7 +6290,7 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="42" t="s">
         <v>173</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -6256,10 +6299,10 @@
       <c r="G18" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="60" t="s">
+      <c r="H18" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="I18" s="61"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="16" t="s">
         <v>179</v>
       </c>
@@ -6271,17 +6314,17 @@
       </c>
     </row>
     <row r="19" spans="5:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="E19" s="66"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="16" t="s">
         <v>174</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="62" t="s">
+      <c r="H19" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="61"/>
+      <c r="I19" s="38"/>
       <c r="J19" s="16" t="s">
         <v>195</v>
       </c>
@@ -6293,7 +6336,7 @@
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="65" t="s">
+      <c r="E20" s="42" t="s">
         <v>199</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -6302,10 +6345,10 @@
       <c r="G20" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="H20" s="60" t="s">
+      <c r="H20" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="I20" s="61"/>
+      <c r="I20" s="38"/>
       <c r="J20" s="16" t="s">
         <v>179</v>
       </c>
@@ -6317,15 +6360,15 @@
       </c>
     </row>
     <row r="21" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="66"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="G21" s="62" t="s">
+      <c r="G21" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="64"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="16" t="s">
         <v>204</v>
       </c>
@@ -6334,12 +6377,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L15"/>
@@ -6355,6 +6392,12 @@
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I15"/>
     <mergeCell ref="L8:L9"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6378,7 +6421,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="69" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -6386,37 +6429,37 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G3" s="68"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="68"/>
+      <c r="G4" s="70"/>
       <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="68"/>
+      <c r="G5" s="70"/>
       <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="68"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="68"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="68"/>
+      <c r="G8" s="70"/>
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
@@ -9503,7 +9546,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9629,7 +9672,7 @@
   <dimension ref="D5:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9817,7 +9860,7 @@
       <c r="G17" s="16"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="71" t="s">
         <v>237</v>
       </c>
       <c r="E20" s="34" t="s">
@@ -9825,13 +9868,13 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="70"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="34" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="71"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="16" t="s">
         <v>240</v>
       </c>
@@ -9850,282 +9893,341 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E29"/>
+  <dimension ref="B1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="138.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="72" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="35"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="E3" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="F3" s="33" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="F4" s="34" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="75"/>
+      <c r="D5" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="34" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="75"/>
+      <c r="D6" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>4</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="2:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="C7" s="76"/>
+      <c r="D7" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="73" t="s">
+      <c r="C8" s="74" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="36" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="16">
         <v>6</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="75"/>
+      <c r="D9" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <v>8</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="16"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="16">
         <v>9</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
         <v>10</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>11</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
         <v>12</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="72" t="s">
+      <c r="F15" s="16"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="35"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="E18" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="F18" s="33" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <v>1</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="E19" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <v>2</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="16">
         <v>3</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="D21" s="16"/>
       <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="16">
         <v>4</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="34" t="s">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="16">
         <v>5</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="16"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <v>6</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <v>7</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="16"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
         <v>8</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="16">
         <v>9</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="16">
         <v>10</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="16">
         <v>11</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D20" r:id="rId1"/>
-    <hyperlink ref="D19" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E8"/>
-    <hyperlink ref="D22" r:id="rId4"/>
-    <hyperlink ref="E5" r:id="rId5"/>
+    <hyperlink ref="E20" r:id="rId1"/>
+    <hyperlink ref="E19" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F8" display="https://l.facebook.com/l.php?u=https%3A%2F%2Fworld.taobao.com%2Fitem%2F546230564665.htm%3Fspm%3Da312a.7700714.0.0.Qx6JBv%23detail&amp;h=ATMvQ0w2pTaQ0KFJK9Mk5PsS_INYF5Rdl3Tah-FGZMCbctGNBS5EeA3kh-jPaCYaVgJG75UKfI90HglB3qVXtBHbcTeGI-QYzIC8U-l-hprMTKhOqMXVjwwARzf"/>
+    <hyperlink ref="E22" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F7" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8" location="detail"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sync_5_6: Initial Spi driver for camera logging data to SDCard
</commit_message>
<xml_diff>
--- a/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
+++ b/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="278">
   <si>
     <t>STT</t>
   </si>
@@ -855,6 +855,18 @@
   </si>
   <si>
     <t>Link to shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 x Motors </t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>https://oscarliang.com/best-osd-quadcopter-fpv-data-on-screen-display-video/</t>
+  </si>
+  <si>
+    <t>OSD</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1160,27 +1172,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1256,6 +1251,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1280,7 +1296,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6155,18 +6170,18 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E6" s="21" t="s">
@@ -6183,15 +6198,15 @@
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="16" t="s">
         <v>179</v>
       </c>
@@ -6203,35 +6218,35 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="58"/>
-      <c r="F8" s="59" t="s">
+      <c r="E8" s="53"/>
+      <c r="F8" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="57" t="s">
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="57" t="s">
+      <c r="K8" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="57" t="s">
+      <c r="L8" s="52" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="54"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="48" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="19" t="s">
@@ -6255,7 +6270,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="58"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="18" t="s">
         <v>161</v>
       </c>
@@ -6277,7 +6292,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="54"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="18" t="s">
         <v>165</v>
       </c>
@@ -6299,47 +6314,47 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="44" t="s">
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="41"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="58"/>
-      <c r="F14" s="59" t="s">
+      <c r="E14" s="53"/>
+      <c r="F14" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="47" t="s">
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="K14" s="48"/>
-      <c r="L14" s="49"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="54"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="47"/>
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="48" t="s">
         <v>171</v>
       </c>
       <c r="F16" s="16" t="s">
@@ -6365,7 +6380,7 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="54"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="16" t="s">
         <v>207</v>
       </c>
@@ -6389,7 +6404,7 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="68" t="s">
         <v>173</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -6398,10 +6413,10 @@
       <c r="G18" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="I18" s="37"/>
+      <c r="I18" s="64"/>
       <c r="J18" s="16" t="s">
         <v>179</v>
       </c>
@@ -6413,17 +6428,17 @@
       </c>
     </row>
     <row r="19" spans="5:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="E19" s="42"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="16" t="s">
         <v>174</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="38" t="s">
+      <c r="H19" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="37"/>
+      <c r="I19" s="64"/>
       <c r="J19" s="16" t="s">
         <v>195</v>
       </c>
@@ -6435,7 +6450,7 @@
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="68" t="s">
         <v>199</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -6444,10 +6459,10 @@
       <c r="G20" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="I20" s="37"/>
+      <c r="I20" s="64"/>
       <c r="J20" s="16" t="s">
         <v>179</v>
       </c>
@@ -6459,15 +6474,15 @@
       </c>
     </row>
     <row r="21" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="42"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="65" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67"/>
       <c r="J21" s="16" t="s">
         <v>204</v>
       </c>
@@ -6476,6 +6491,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L15"/>
@@ -6491,12 +6512,6 @@
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I15"/>
     <mergeCell ref="L8:L9"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6520,7 +6535,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="70" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -6528,37 +6543,37 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G3" s="69"/>
+      <c r="G3" s="71"/>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="69"/>
+      <c r="G4" s="71"/>
       <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="69"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="69"/>
+      <c r="G6" s="71"/>
       <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="69"/>
+      <c r="G7" s="71"/>
       <c r="H7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="69"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
@@ -9959,7 +9974,7 @@
       <c r="G17" s="16"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="70" t="s">
+      <c r="D20" s="72" t="s">
         <v>237</v>
       </c>
       <c r="E20" s="34" t="s">
@@ -9967,13 +9982,13 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="71"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="34" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="72"/>
+      <c r="D22" s="74"/>
       <c r="E22" s="16" t="s">
         <v>240</v>
       </c>
@@ -9994,8 +10009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10038,7 +10053,7 @@
       <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="75" t="s">
         <v>262</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -10056,7 +10071,7 @@
       <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="74"/>
+      <c r="C5" s="76"/>
       <c r="D5" s="16" t="s">
         <v>258</v>
       </c>
@@ -10070,7 +10085,7 @@
       <c r="B6" s="16">
         <v>3</v>
       </c>
-      <c r="C6" s="74"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="16" t="s">
         <v>264</v>
       </c>
@@ -10080,7 +10095,7 @@
       <c r="F6" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G6" s="76" t="s">
+      <c r="G6" s="37" t="s">
         <v>272</v>
       </c>
     </row>
@@ -10088,7 +10103,7 @@
       <c r="B7" s="16">
         <v>4</v>
       </c>
-      <c r="C7" s="75"/>
+      <c r="C7" s="77"/>
       <c r="D7" s="16" t="s">
         <v>266</v>
       </c>
@@ -10104,7 +10119,7 @@
       <c r="B8" s="16">
         <v>5</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="75" t="s">
         <v>263</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -10120,7 +10135,7 @@
       <c r="B9" s="16">
         <v>6</v>
       </c>
-      <c r="C9" s="74"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="16" t="s">
         <v>270</v>
       </c>
@@ -10136,7 +10151,7 @@
       <c r="B10" s="16">
         <v>7</v>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -10146,7 +10161,7 @@
       <c r="B11" s="16">
         <v>8</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -10156,8 +10171,12 @@
       <c r="B12" s="16">
         <v>9</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="75" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>274</v>
+      </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -10166,20 +10185,24 @@
       <c r="B13" s="16">
         <v>10</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="16"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>11</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="36" t="s">
+        <v>277</v>
+      </c>
       <c r="D14" s="34"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="F14" s="34" t="s">
+        <v>276</v>
+      </c>
       <c r="G14" s="16"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -10329,9 +10352,10 @@
       <c r="F29" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1"/>
@@ -10344,9 +10368,10 @@
     <hyperlink ref="F7" r:id="rId7"/>
     <hyperlink ref="F9" r:id="rId8" location="detail"/>
     <hyperlink ref="G6" r:id="rId9"/>
+    <hyperlink ref="F14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sync 11_6: Update docs
</commit_message>
<xml_diff>
--- a/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
+++ b/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="510" windowWidth="19875" windowHeight="7275" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="510" windowWidth="19875" windowHeight="7275" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="RawIdeaAnalysis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="285">
   <si>
     <t>STT</t>
   </si>
@@ -799,9 +799,6 @@
     <t>970.000 VND</t>
   </si>
   <si>
-    <t>https://l.facebook.com/l.php?u=https%3A%2F%2Fworld.taobao.com%2Fitem%2F546230564665.htm%3Fspm%3Da312a.7700714.0.0.Qx6JBv%23detail&amp;h=ATMvQ0w2pTaQ0KFJK9Mk5PsS_INYF5Rdl3Tah-FGZMCbctGNBS5EeA3kh-jPaCYaVgJG75UKfI90HglB3qVXtBHbcTeGI-QYzIC8U-l-hprMTKhOqMXVjwwARzfwHK7SJhiQkvdlQg</t>
-  </si>
-  <si>
     <t>https://oscarliang.com/mini-quad-not-blackout-qav250/</t>
   </si>
   <si>
@@ -867,6 +864,30 @@
   </si>
   <si>
     <t>OSD</t>
+  </si>
+  <si>
+    <t>https://oscarliang.com/best-looptime-flight-controller/</t>
+  </si>
+  <si>
+    <t>Loop time to sample sensor</t>
+  </si>
+  <si>
+    <t>http://quanphongrc.vn/ct/may-bay-dieu-khien/224/devo-7e-without-rx-khong-bao-gom-rx.html</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Devo 7E (Without RX - không bao gồm RX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 900.000 VND</t>
+  </si>
+  <si>
+    <t>http://www.clbmohinh.com/forum/m1348891-print.aspx</t>
+  </si>
+  <si>
+    <t>CC3D Evo</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1172,10 +1193,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1251,27 +1293,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1294,6 +1315,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5694,13 +5724,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>802821</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>5137273</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>170868</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5732,7 +5762,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>830037</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3429080" cy="374141"/>
@@ -6170,18 +6200,18 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E6" s="21" t="s">
@@ -6198,15 +6228,15 @@
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="16" t="s">
         <v>179</v>
       </c>
@@ -6218,35 +6248,35 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="53"/>
-      <c r="F8" s="54" t="s">
+      <c r="E8" s="60"/>
+      <c r="F8" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="52" t="s">
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="L8" s="52" t="s">
+      <c r="L8" s="59" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="49"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="55" t="s">
         <v>169</v>
       </c>
       <c r="F10" s="19" t="s">
@@ -6270,7 +6300,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="53"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="18" t="s">
         <v>161</v>
       </c>
@@ -6292,7 +6322,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="49"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="18" t="s">
         <v>165</v>
       </c>
@@ -6314,47 +6344,47 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="60" t="s">
+      <c r="F13" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="39" t="s">
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="40"/>
-      <c r="L13" s="41"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="53"/>
-      <c r="F14" s="54" t="s">
+      <c r="E14" s="60"/>
+      <c r="F14" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="42" t="s">
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="49"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="47"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="54"/>
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="55" t="s">
         <v>171</v>
       </c>
       <c r="F16" s="16" t="s">
@@ -6380,7 +6410,7 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="49"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="16" t="s">
         <v>207</v>
       </c>
@@ -6404,7 +6434,7 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="68" t="s">
+      <c r="E18" s="43" t="s">
         <v>173</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -6413,10 +6443,10 @@
       <c r="G18" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="I18" s="64"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="16" t="s">
         <v>179</v>
       </c>
@@ -6428,17 +6458,17 @@
       </c>
     </row>
     <row r="19" spans="5:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="E19" s="69"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="16" t="s">
         <v>174</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="H19" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="64"/>
+      <c r="I19" s="39"/>
       <c r="J19" s="16" t="s">
         <v>195</v>
       </c>
@@ -6450,7 +6480,7 @@
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="43" t="s">
         <v>199</v>
       </c>
       <c r="F20" s="16" t="s">
@@ -6459,10 +6489,10 @@
       <c r="G20" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="H20" s="63" t="s">
+      <c r="H20" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="I20" s="64"/>
+      <c r="I20" s="39"/>
       <c r="J20" s="16" t="s">
         <v>179</v>
       </c>
@@ -6474,15 +6504,15 @@
       </c>
     </row>
     <row r="21" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="69"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="G21" s="65" t="s">
+      <c r="G21" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="66"/>
-      <c r="I21" s="67"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
       <c r="J21" s="16" t="s">
         <v>204</v>
       </c>
@@ -6491,12 +6521,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L15"/>
@@ -6512,6 +6536,12 @@
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I15"/>
     <mergeCell ref="L8:L9"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9785,8 +9815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10007,15 +10037,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G29"/>
+  <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="C19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="80" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="91.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
@@ -10024,17 +10054,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="78" t="s">
         <v>244</v>
       </c>
       <c r="C1" s="35"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="79" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>216</v>
@@ -10043,18 +10073,18 @@
         <v>253</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G3" s="33" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="16">
+      <c r="B4" s="37">
         <v>1</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>252</v>
@@ -10068,310 +10098,412 @@
       <c r="G4" s="16"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
+      <c r="B5" s="37">
         <v>2</v>
       </c>
       <c r="C5" s="76"/>
       <c r="D5" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="37">
         <v>3</v>
       </c>
       <c r="C6" s="76"/>
       <c r="D6" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>265</v>
-      </c>
       <c r="F6" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>272</v>
+        <v>259</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="37">
         <v>4</v>
       </c>
       <c r="C7" s="77"/>
       <c r="D7" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>267</v>
-      </c>
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="75">
         <v>5</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="16"/>
-      <c r="F8" s="16" t="s">
-        <v>255</v>
-      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
-        <v>6</v>
-      </c>
+      <c r="B9" s="76"/>
       <c r="C9" s="76"/>
       <c r="D9" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>271</v>
-      </c>
       <c r="F9" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G9" s="16"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
-        <v>7</v>
-      </c>
+      <c r="B10" s="76"/>
       <c r="C10" s="76"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
-        <v>8</v>
-      </c>
-      <c r="C11" s="77"/>
+    <row r="11" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
-        <v>9</v>
-      </c>
-      <c r="C12" s="75" t="s">
-        <v>275</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>274</v>
-      </c>
+    <row r="12" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
-        <v>10</v>
-      </c>
+      <c r="B13" s="77"/>
       <c r="C13" s="77"/>
-      <c r="D13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>284</v>
+      </c>
       <c r="E13" s="16"/>
-      <c r="F13" s="34"/>
+      <c r="F13" s="34" t="s">
+        <v>283</v>
+      </c>
       <c r="G13" s="16"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <v>11</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>277</v>
-      </c>
-      <c r="D14" s="34"/>
+      <c r="B14" s="75">
+        <v>6</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>273</v>
+      </c>
       <c r="E14" s="16"/>
-      <c r="F14" s="34" t="s">
-        <v>276</v>
-      </c>
+      <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
-        <v>12</v>
-      </c>
-      <c r="C15" s="16"/>
+    <row r="15" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="C17" s="35"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
-        <v>1</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
-        <v>2</v>
-      </c>
-      <c r="C20" s="16"/>
+    <row r="16" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="75">
+        <v>7</v>
+      </c>
+      <c r="C18" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="75">
+        <v>8</v>
+      </c>
+      <c r="C20" s="75" t="s">
+        <v>280</v>
+      </c>
       <c r="D20" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="16">
-        <v>3</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
-        <v>248</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="16">
-        <v>4</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
-        <v>5</v>
-      </c>
-      <c r="C23" s="16"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="16">
-        <v>6</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
-        <v>7</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="16"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
-        <v>8</v>
-      </c>
-      <c r="C26" s="16"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
+      <c r="F26" s="34"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="78" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="35"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="37">
+        <v>1</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="37">
+        <v>2</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="37">
+        <v>3</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="37">
+        <v>4</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="37">
+        <v>5</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="37">
+        <v>6</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="37">
+        <v>7</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="37">
+        <v>8</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="37">
         <v>9</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="16">
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="37">
         <v>10</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="16">
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="37">
         <v>11</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
     <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B20:B23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E20" r:id="rId1"/>
-    <hyperlink ref="E19" r:id="rId2"/>
+    <hyperlink ref="E31" r:id="rId1"/>
+    <hyperlink ref="E30" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F8" display="https://l.facebook.com/l.php?u=https%3A%2F%2Fworld.taobao.com%2Fitem%2F546230564665.htm%3Fspm%3Da312a.7700714.0.0.Qx6JBv%23detail&amp;h=ATMvQ0w2pTaQ0KFJK9Mk5PsS_INYF5Rdl3Tah-FGZMCbctGNBS5EeA3kh-jPaCYaVgJG75UKfI90HglB3qVXtBHbcTeGI-QYzIC8U-l-hprMTKhOqMXVjwwARzf"/>
-    <hyperlink ref="E22" r:id="rId4"/>
+    <hyperlink ref="E33" r:id="rId4"/>
     <hyperlink ref="F5" r:id="rId5"/>
     <hyperlink ref="F6" r:id="rId6"/>
     <hyperlink ref="F7" r:id="rId7"/>
     <hyperlink ref="F9" r:id="rId8" location="detail"/>
     <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
+    <hyperlink ref="E34" r:id="rId10"/>
+    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F18" r:id="rId12"/>
+    <hyperlink ref="F20" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
-  <drawing r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sync 18_6: Update docs
</commit_message>
<xml_diff>
--- a/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
+++ b/Docs/Design_Arch/BL_SW_FLATFORM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="510" windowWidth="19875" windowHeight="7275" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="570" windowWidth="19875" windowHeight="7215" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="RawIdeaAnalysis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="299">
   <si>
     <t>STT</t>
   </si>
@@ -884,9 +884,6 @@
     <t xml:space="preserve"> 900.000 VND</t>
   </si>
   <si>
-    <t>http://www.clbmohinh.com/forum/m1348891-print.aspx</t>
-  </si>
-  <si>
     <t>CC3D Evo</t>
   </si>
   <si>
@@ -900,6 +897,40 @@
   </si>
   <si>
     <t>How to Choose A Sensible Sampling Rate</t>
+  </si>
+  <si>
+    <t>https://oscarliang.com/3s-4s-setup-mini-quadcopter/</t>
+  </si>
+  <si>
+    <t>Mini Quad: 3S, 4S Setups Comparison and Migration</t>
+  </si>
+  <si>
+    <t>http://www.clbmohinh.com/forum/m1348891-print.aspx
+http://quanphongrc.vn/ct/chi-tiet/260/cc3d.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 330.000 VND </t>
+  </si>
+  <si>
+    <t>http://quanphongrc.vn/ct/may-bay-dieu-khien/1270/emax-rs2205-s-2300kv-racespec-motor-cooling-series-for-fpv-multicopter-4pcs-set.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.240.000 VND </t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>http://quanphongrc.vn/ct/may-bay-dieu-khien/1561/4x-favourite-fvt-littlebee-30a-s-esc-blheli-s-opto-2-6s-supports-mulitshot-oneshot42-oneshot125.html</t>
+  </si>
+  <si>
+    <t>4X Favourite FVT LittleBee 30A-S ESC BLHeli_S OPTO 2-6S Supports Mulitshot Oneshot42 OneShot125</t>
+  </si>
+  <si>
+    <t>1.200.000 VND</t>
+  </si>
+  <si>
+    <t>RX</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1338,6 +1369,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5734,16 +5768,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>802821</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>5137273</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>170868</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>486105</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>29850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5760,8 +5794,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1415142" y="6572249"/>
-          <a:ext cx="6266667" cy="4647619"/>
+          <a:off x="26297659" y="5669231"/>
+          <a:ext cx="6261719" cy="4647619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5772,10 +5806,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>830037</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>293172</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>32162</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3429080" cy="374141"/>
     <xdr:sp macro="" textlink="">
@@ -5785,7 +5819,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1442358" y="6041571"/>
+          <a:off x="26305081" y="4985162"/>
           <a:ext cx="3429080" cy="374141"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5817,6 +5851,80 @@
             <a:rPr lang="en-US" sz="1800" b="1"/>
             <a:t>DALRC DL265 FPV Quad Frame Kit</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>54552</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="12312794" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="682337" y="8055552"/>
+          <a:ext cx="12312794" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Cấu</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> hình Robocat</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Cấu hình robocat Kit robocat 650k Fc f3 330k Bec 5in1 168k Esc Favourite FVT LittleBee 30A-S 1200k Motor EMAX RS2205-S 2300KV 1240k Led 192k Chân TAROT 52k Cánh kingkong 5045 32k Pin tattu 2s 1800mah</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10051,16 +10159,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="91.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="138.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -10209,15 +10317,17 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="80"/>
       <c r="C13" s="80"/>
       <c r="D13" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="34" t="s">
         <v>283</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="F13" s="81" t="s">
+        <v>290</v>
       </c>
       <c r="G13" s="16"/>
     </row>
@@ -10231,8 +10341,12 @@
       <c r="D14" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>292</v>
+      </c>
       <c r="G14" s="16"/>
     </row>
     <row r="15" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -10324,87 +10438,98 @@
       <c r="G23" s="16"/>
     </row>
     <row r="24" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="78">
+        <v>9</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>295</v>
+      </c>
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="34"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="34"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="16"/>
+    <row r="26" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37">
+        <v>10</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="D26" s="34"/>
       <c r="E26" s="16"/>
       <c r="F26" s="34"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="C28" s="35"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="C29" s="35"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33" t="s">
+      <c r="C30" s="33"/>
+      <c r="D30" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E30" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F30" s="33" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="37">
-        <v>1</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="E30" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="F31" s="16"/>
+        <v>249</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="E32" s="16"/>
+        <v>247</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>245</v>
+      </c>
       <c r="F32" s="16"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -10439,10 +10564,10 @@
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F35" s="16"/>
     </row>
@@ -10452,10 +10577,10 @@
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F36" s="6"/>
     </row>
@@ -10464,8 +10589,12 @@
         <v>8</v>
       </c>
       <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
+      <c r="D37" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>288</v>
+      </c>
       <c r="F37" s="16"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -10496,9 +10625,11 @@
       <c r="F40" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="C14:C17"/>
@@ -10508,8 +10639,8 @@
     <mergeCell ref="B14:B17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E31" r:id="rId1"/>
-    <hyperlink ref="E30" r:id="rId2"/>
+    <hyperlink ref="E32" r:id="rId1"/>
+    <hyperlink ref="E31" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
     <hyperlink ref="E33" r:id="rId4"/>
     <hyperlink ref="F5" r:id="rId5"/>
@@ -10518,14 +10649,17 @@
     <hyperlink ref="F9" r:id="rId8" location="detail"/>
     <hyperlink ref="G6" r:id="rId9"/>
     <hyperlink ref="E34" r:id="rId10"/>
-    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId11" display="http://www.clbmohinh.com/forum/m1348891-print.aspx"/>
     <hyperlink ref="F18" r:id="rId12"/>
     <hyperlink ref="F20" r:id="rId13"/>
     <hyperlink ref="E35" r:id="rId14"/>
     <hyperlink ref="E36" r:id="rId15"/>
+    <hyperlink ref="E37" r:id="rId16"/>
+    <hyperlink ref="F14" r:id="rId17"/>
+    <hyperlink ref="F24" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
-  <drawing r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>